<commit_message>
added the register user function
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,12 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t xml:space="preserve">Username</t>
   </si>
   <si>
-    <t xml:space="preserve">Password</t>
+    <t xml:space="preserve">Passwort</t>
   </si>
   <si>
     <t xml:space="preserve">DisplayName</t>
@@ -34,40 +34,49 @@
     <t xml:space="preserve">Alter</t>
   </si>
   <si>
-    <t xml:space="preserve">ReferenzZuAvatar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fitness Level /100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LäuftLos?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Position</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zeit</t>
+    <t xml:space="preserve">FelixSwimmer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">passwort123</t>
   </si>
   <si>
     <t xml:space="preserve">Mezix</t>
   </si>
   <si>
-    <t xml:space="preserve">passwort123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FelixSwimmer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avatar1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nein</t>
-  </si>
-  <si>
-    <t xml:space="preserve">null</t>
-  </si>
-  <si>
-    <t>TEST</t>
+    <t xml:space="preserve">21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">werbrauchtdenpasswörter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Josephine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">keinbockmehr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hande</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blabla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hande</t>
+  </si>
+  <si>
+    <t xml:space="preserve">456</t>
   </si>
 </sst>
 </file>
@@ -101,7 +110,7 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="10"/>
+      <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -115,19 +124,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -161,11 +163,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -186,80 +188,91 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="14.59" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="17.78" collapsed="true" outlineLevel="0"/>
-    <col min="6" max="6" customWidth="true" hidden="false" style="0" width="20.98" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="36.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="35.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.98"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="11.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2" t="n">
-        <v>21</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="2" t="n">
-        <v>50</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the login feature
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,63 +20,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+  <si>
+    <t xml:space="preserve">First Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age</t>
+  </si>
   <si>
     <t xml:space="preserve">Username</t>
   </si>
   <si>
-    <t xml:space="preserve">Passwort</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DisplayName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FelixSwimmer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">passwort123</t>
+    <t xml:space="preserve">Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Felixsss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swimmer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21</t>
   </si>
   <si>
     <t xml:space="preserve">Mezix</t>
   </si>
   <si>
-    <t xml:space="preserve">21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enric</t>
-  </si>
-  <si>
-    <t xml:space="preserve">werbrauchtdenpasswörter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Josephine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">keinbockmehr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hande</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blabla</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hande</t>
-  </si>
-  <si>
-    <t xml:space="preserve">456</t>
+    <t xml:space="preserve">passwort</t>
+  </si>
+  <si>
+    <t>Felixsss</t>
+  </si>
+  <si>
+    <t>Swimmer</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>Mezix2</t>
+  </si>
+  <si>
+    <t>passwort</t>
   </si>
 </sst>
 </file>
@@ -124,12 +112,19 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -167,7 +162,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -188,21 +183,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="36.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="35.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.98"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="11.67"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="36.54" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="31.68" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="9.03" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="27.92" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="1" width="47.93" collapsed="true" outlineLevel="0"/>
+    <col min="6" max="6" customWidth="true" hidden="false" style="1" width="20.98" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="1025" customWidth="false" hidden="false" style="1" width="11.67" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -218,61 +213,42 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
+    <row r="3">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E3" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed some bugs and returned strings
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t xml:space="preserve">Username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password</t>
+  </si>
   <si>
     <t xml:space="preserve">First Name</t>
   </si>
@@ -31,40 +37,19 @@
     <t xml:space="preserve">Age</t>
   </si>
   <si>
-    <t xml:space="preserve">Username</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Felixsss</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Swimmer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mezix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">passwort</t>
-  </si>
-  <si>
-    <t>Felixsss</t>
+    <t>Mezix</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Felix</t>
   </si>
   <si>
     <t>Swimmer</t>
   </si>
   <si>
     <t>21</t>
-  </si>
-  <si>
-    <t>Mezix2</t>
-  </si>
-  <si>
-    <t>passwort</t>
   </si>
 </sst>
 </file>
@@ -183,19 +168,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" customWidth="true" hidden="false" style="1" width="36.54" collapsed="true" outlineLevel="0"/>
     <col min="2" max="2" customWidth="true" hidden="false" style="1" width="31.68" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="9.03" collapsed="true" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="27.92" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="1" width="47.93" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="30.97" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="31.12" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="1" width="8.75" collapsed="true" outlineLevel="0"/>
     <col min="6" max="6" customWidth="true" hidden="false" style="1" width="20.98" collapsed="true" outlineLevel="0"/>
     <col min="7" max="1025" customWidth="false" hidden="false" style="1" width="11.67" collapsed="true" outlineLevel="0"/>
   </cols>
@@ -217,38 +202,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the ability to remove friends
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t xml:space="preserve">Username</t>
   </si>
@@ -37,27 +37,58 @@
     <t xml:space="preserve">Age</t>
   </si>
   <si>
-    <t>Mezix</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>Felix</t>
-  </si>
-  <si>
-    <t>Swimmer</t>
-  </si>
-  <si>
-    <t>21</t>
+    <t xml:space="preserve">FreundesListe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fitness Level (X/100)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Läuft los</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lauf Start Position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zeit des Laufs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mezix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Felix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swimmer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enric;Phine;Mezix2;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mezix2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enric</t>
+  </si>
+  <si>
+    <t>Phine;Mezix2;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -138,7 +169,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -148,6 +179,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -168,10 +203,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -181,8 +216,12 @@
     <col min="3" max="3" customWidth="true" hidden="false" style="1" width="30.97" collapsed="true" outlineLevel="0"/>
     <col min="4" max="4" customWidth="true" hidden="false" style="1" width="31.12" collapsed="true" outlineLevel="0"/>
     <col min="5" max="5" customWidth="true" hidden="false" style="1" width="8.75" collapsed="true" outlineLevel="0"/>
-    <col min="6" max="6" customWidth="true" hidden="false" style="1" width="20.98" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="1025" customWidth="false" hidden="false" style="1" width="11.67" collapsed="true" outlineLevel="0"/>
+    <col min="6" max="6" customWidth="true" hidden="false" style="1" width="17.92" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="7" customWidth="true" hidden="false" style="1" width="23.35" collapsed="true" outlineLevel="0"/>
+    <col min="8" max="8" customWidth="true" hidden="false" style="1" width="15.68" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="22.36" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="21.56" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="1025" customWidth="false" hidden="false" style="1" width="11.67" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -201,22 +240,74 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added getAllInfo and start stop run methods
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t xml:space="preserve">Username</t>
   </si>
@@ -40,16 +40,16 @@
     <t xml:space="preserve">FreundesListe</t>
   </si>
   <si>
-    <t xml:space="preserve">Fitness Level (X/100)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Läuft los</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lauf Start Position</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zeit des Laufs</t>
+    <t xml:space="preserve">LaufStatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LaufStartPos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laufzeit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FitnessLevel</t>
   </si>
   <si>
     <t xml:space="preserve">Mezix</t>
@@ -67,7 +67,10 @@
     <t xml:space="preserve">21</t>
   </si>
   <si>
-    <t xml:space="preserve">Enric;Phine;Mezix2;</t>
+    <t xml:space="preserve">Phine;Mezix2;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">false</t>
   </si>
   <si>
     <t xml:space="preserve">Mezix2</t>
@@ -79,16 +82,27 @@
     <t xml:space="preserve">Enric</t>
   </si>
   <si>
-    <t>Phine;Mezix2;</t>
+    <t>false</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>lat/lng: (53.6175727,9.8987057)</t>
+  </si>
+  <si>
+    <t>14:23</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -169,7 +183,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -179,10 +193,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -206,7 +216,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -217,10 +227,10 @@
     <col min="4" max="4" customWidth="true" hidden="false" style="1" width="31.12" collapsed="true" outlineLevel="0"/>
     <col min="5" max="5" customWidth="true" hidden="false" style="1" width="8.75" collapsed="true" outlineLevel="0"/>
     <col min="6" max="6" customWidth="true" hidden="false" style="1" width="17.92" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="7" customWidth="true" hidden="false" style="1" width="23.35" collapsed="true" outlineLevel="0"/>
-    <col min="8" max="8" customWidth="true" hidden="false" style="1" width="15.68" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="22.36" collapsed="true" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="21.56" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="7" customWidth="true" hidden="false" style="1" width="12.5" collapsed="true" outlineLevel="0"/>
+    <col min="8" max="8" customWidth="true" hidden="false" style="1" width="32.22" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="9.72" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="14.43" collapsed="true" outlineLevel="0"/>
     <col min="11" max="1025" customWidth="false" hidden="false" style="1" width="11.67" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
@@ -272,20 +282,22 @@
       <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="H2" s="3" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
@@ -302,12 +314,12 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed login and register to initialise all fields!
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
   <si>
     <t xml:space="preserve">Username</t>
   </si>
@@ -67,22 +67,19 @@
     <t xml:space="preserve">21</t>
   </si>
   <si>
+    <t xml:space="preserve">END</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carsten</t>
+  </si>
+  <si>
     <t xml:space="preserve">false</t>
   </si>
   <si>
-    <t xml:space="preserve">hello</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">END</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enric</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carsten</t>
+    <t xml:space="preserve">0</t>
   </si>
   <si>
     <t xml:space="preserve">Phine</t>
@@ -98,16 +95,20 @@
   </si>
   <si>
     <t xml:space="preserve">Eyicalis</t>
+  </si>
+  <si>
+    <t>false</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -135,6 +136,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -186,7 +192,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -196,6 +202,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -219,22 +233,22 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="36.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="31.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="32.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="11.67"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="36.54" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="31.68" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="30.97" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="31.12" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="1" width="8.75" collapsed="true" outlineLevel="0"/>
+    <col min="6" max="6" customWidth="true" hidden="false" style="1" width="17.92" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="7" customWidth="true" hidden="false" style="1" width="12.5" collapsed="true" outlineLevel="0"/>
+    <col min="8" max="8" customWidth="true" hidden="false" style="1" width="32.22" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="9.72" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="14.43" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="1025" customWidth="false" hidden="false" style="1" width="11.67" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -285,77 +299,92 @@
       <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="G3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="K3" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="G4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="K4" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="G5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="K5" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
formatted fitnesslevel as text
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t xml:space="preserve">Username</t>
   </si>
@@ -67,6 +67,9 @@
     <t xml:space="preserve">21</t>
   </si>
   <si>
+    <t xml:space="preserve">false</t>
+  </si>
+  <si>
     <t xml:space="preserve">END</t>
   </si>
   <si>
@@ -76,9 +79,6 @@
     <t xml:space="preserve">Carsten</t>
   </si>
   <si>
-    <t xml:space="preserve">false</t>
-  </si>
-  <si>
     <t xml:space="preserve">0</t>
   </si>
   <si>
@@ -95,9 +95,6 @@
   </si>
   <si>
     <t xml:space="preserve">Eyicalis</t>
-  </si>
-  <si>
-    <t>false</t>
   </si>
 </sst>
 </file>
@@ -106,9 +103,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -136,11 +133,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -192,7 +184,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -205,11 +197,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -233,22 +221,22 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="36.54" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="31.68" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="30.97" collapsed="true" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="31.12" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="1" width="8.75" collapsed="true" outlineLevel="0"/>
-    <col min="6" max="6" customWidth="true" hidden="false" style="1" width="17.92" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="7" customWidth="true" hidden="false" style="1" width="12.5" collapsed="true" outlineLevel="0"/>
-    <col min="8" max="8" customWidth="true" hidden="false" style="1" width="32.22" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="9.72" collapsed="true" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="14.43" collapsed="true" outlineLevel="0"/>
-    <col min="11" max="1025" customWidth="false" hidden="false" style="1" width="11.67" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="36.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="31.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="32.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="11.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -299,40 +287,40 @@
       <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="4" t="n">
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="3" t="n">
         <v>0</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>19</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -352,13 +340,13 @@
         <v>14</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>19</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -378,13 +366,13 @@
         <v>14</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>19</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the ability to scan our area for people starting a run, using the username and a max distance
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
   <si>
     <t xml:space="preserve">Username</t>
   </si>
@@ -67,7 +67,13 @@
     <t xml:space="preserve">21</t>
   </si>
   <si>
-    <t xml:space="preserve">false</t>
+    <t xml:space="preserve">true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lat/lng: (53.6175727,9.8987057)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:23</t>
   </si>
   <si>
     <t xml:space="preserve">0</t>
@@ -91,10 +97,16 @@
     <t xml:space="preserve">Siems</t>
   </si>
   <si>
+    <t xml:space="preserve">lat/lng: (53.7175727,9.8987057)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hande</t>
   </si>
   <si>
     <t xml:space="preserve">Eyicalis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lat/lng: (12.6175727,9.8987057)</t>
   </si>
 </sst>
 </file>
@@ -216,7 +228,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -285,25 +297,31 @@
       <c r="G2" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="J2" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>14</v>
@@ -311,25 +329,28 @@
       <c r="G3" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="H3" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="J3" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>14</v>
@@ -337,25 +358,28 @@
       <c r="G4" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="H4" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="J4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
@@ -363,11 +387,14 @@
       <c r="G5" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="H5" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="J5" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed the names of commands
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="76">
   <si>
     <t xml:space="preserve">Username</t>
   </si>
@@ -70,6 +70,9 @@
     <t xml:space="preserve">Gewicht</t>
   </si>
   <si>
+    <t xml:space="preserve">Activity Type</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mezix</t>
   </si>
   <si>
@@ -97,6 +100,9 @@
     <t xml:space="preserve">0</t>
   </si>
   <si>
+    <t xml:space="preserve">run</t>
+  </si>
+  <si>
     <t xml:space="preserve">END</t>
   </si>
   <si>
@@ -118,57 +124,63 @@
     <t xml:space="preserve">Siems</t>
   </si>
   <si>
+    <t xml:space="preserve">false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hande</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eyicalis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mezix;Enric;Hande;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lat/lng: (12.6175727,9.8987057)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lat/lng: (58.6175727,9.8987057)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lat/lng: (52.6175727,9.087057)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aaa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lat/lng: (58.7155727,9.89870507)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aaaa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lat/lng: (12.61275727,9.8987057)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aaaaa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aaaaaa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lat/lng: (54.6175727,9.5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aaaaaaa</t>
+  </si>
+  <si>
     <t xml:space="preserve">lat/lng: (53.7175727,9.8987057)</t>
   </si>
   <si>
-    <t xml:space="preserve">Hande</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eyicalis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mezix;Enric;Hande;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lat/lng: (12.6175727,9.8987057)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lat/lng: (58.6175727,9.8987057)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lat/lng: (52.6175727,9.087057)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aaa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lat/lng: (58.7155727,9.89870507)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aaaa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lat/lng: (12.61275727,9.8987057)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aaaaa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aaaaaa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lat/lng: (54.6175727,9.5)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aaaaaaa</t>
-  </si>
-  <si>
     <t xml:space="preserve">aaaaaaaa</t>
   </si>
   <si>
@@ -236,15 +248,6 @@
   </si>
   <si>
     <t xml:space="preserve">aaaaaaaaaaaaaaaaaaaaaaaa</t>
-  </si>
-  <si>
-    <t>Phine;</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>false</t>
   </si>
 </sst>
 </file>
@@ -374,28 +377,30 @@
   </sheetPr>
   <dimension ref="A1:AY35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M27" activeCellId="0" sqref="M27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q9" activeCellId="0" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="36.54" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="31.68" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="30.97" collapsed="true" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="31.12" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="1" width="8.75" collapsed="true" outlineLevel="0"/>
-    <col min="6" max="6" customWidth="true" hidden="false" style="1" width="17.92" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="7" customWidth="true" hidden="false" style="1" width="16.87" collapsed="true" outlineLevel="0"/>
-    <col min="8" max="8" customWidth="true" hidden="false" style="1" width="32.22" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="21.95" collapsed="true" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="14.43" collapsed="true" outlineLevel="0"/>
-    <col min="11" max="11" customWidth="true" hidden="false" style="1" width="14.21" collapsed="true" outlineLevel="0"/>
-    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="17.52" collapsed="true" outlineLevel="0"/>
-    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="18.77" collapsed="true" outlineLevel="0"/>
-    <col min="14" max="14" customWidth="true" hidden="false" style="1" width="16.81" collapsed="true" outlineLevel="0"/>
-    <col min="15" max="15" customWidth="true" hidden="false" style="1" width="23.76" collapsed="true" outlineLevel="0"/>
-    <col min="16" max="1025" customWidth="false" hidden="false" style="1" width="11.67" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="36.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="31.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="32.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="21.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="14.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="17.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="18.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="23.76"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="11.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="15.18"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="18" style="1" width="11.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -447,7 +452,9 @@
       <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3"/>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="R1" s="3"/>
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
@@ -463,813 +470,957 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K2" s="0"/>
       <c r="N2" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="AY2" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" t="s">
-        <v>73</v>
+        <v>30</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="K3" s="0"/>
       <c r="N3" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="AY3" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" t="s">
-        <v>74</v>
-      </c>
-      <c r="H4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I4" t="s">
-        <v>73</v>
-      </c>
-      <c r="J4" t="s">
-        <v>73</v>
+        <v>21</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="K4" s="0"/>
       <c r="N4" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="AY4" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="K5" s="0"/>
       <c r="N5" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="AY5" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N6" s="4" t="s">
-        <v>24</v>
+      <c r="N6" s="4"/>
+      <c r="Q6" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="AY6" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>32</v>
+        <v>52</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>32</v>
+        <v>52</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>32</v>
+        <v>52</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>32</v>
+        <v>52</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N31" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="N31" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N32" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="N32" s="4"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N33" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="N33" s="4"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N34" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="N34" s="4"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N35" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="N35" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
added the ability to process medals
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="86">
   <si>
     <t xml:space="preserve">Username</t>
   </si>
@@ -73,6 +73,9 @@
     <t xml:space="preserve">Activity Type</t>
   </si>
   <si>
+    <t xml:space="preserve">TimeWhenLastActivityStarted</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mezix</t>
   </si>
   <si>
@@ -97,6 +100,9 @@
     <t xml:space="preserve">14:23</t>
   </si>
   <si>
+    <t xml:space="preserve">runningrain;3_5streak;2_10streak;1_</t>
+  </si>
+  <si>
     <t xml:space="preserve">0</t>
   </si>
   <si>
@@ -127,6 +133,9 @@
     <t xml:space="preserve">false</t>
   </si>
   <si>
+    <t xml:space="preserve">lat/lng: (57.6175727,9.87987057)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hande</t>
   </si>
   <si>
@@ -142,7 +151,7 @@
     <t xml:space="preserve">a</t>
   </si>
   <si>
-    <t xml:space="preserve">lat/lng: (58.6175727,9.8987057)</t>
+    <t xml:space="preserve">lat/lng: (58.6175727,10.8987057)</t>
   </si>
   <si>
     <t xml:space="preserve">bike</t>
@@ -151,7 +160,7 @@
     <t xml:space="preserve">aa</t>
   </si>
   <si>
-    <t xml:space="preserve">lat/lng: (52.6175727,9.087057)</t>
+    <t xml:space="preserve">lat/lng: (52.6175727,15.087057)</t>
   </si>
   <si>
     <t xml:space="preserve">aaa</t>
@@ -196,25 +205,31 @@
     <t xml:space="preserve">aaaaaaaaaa</t>
   </si>
   <si>
-    <t xml:space="preserve">lat/lng: (54.6175727,9.87987057)</t>
+    <t xml:space="preserve">lat/lng: (54.6175727,6.87987057)</t>
   </si>
   <si>
     <t xml:space="preserve">aaaaaaaaaaa</t>
   </si>
   <si>
+    <t xml:space="preserve">lat/lng: (53.7175727,2.8987057)</t>
+  </si>
+  <si>
     <t xml:space="preserve">aaaaaaaaaaaa</t>
   </si>
   <si>
+    <t xml:space="preserve">lat/lng: (12.6175727,1.8987057)</t>
+  </si>
+  <si>
     <t xml:space="preserve">aaaaaaaaaaaaa</t>
   </si>
   <si>
-    <t xml:space="preserve">lat/lng: (2.6175727,9.8987057)</t>
+    <t xml:space="preserve">lat/lng: (2.6175727,19.8987057)</t>
   </si>
   <si>
     <t xml:space="preserve">aaaaaaaaaaaaaaa</t>
   </si>
   <si>
-    <t xml:space="preserve">lat/lng: (84.6175727,9.8987057)</t>
+    <t xml:space="preserve">lat/lng: (84.6175727,0.8987057)</t>
   </si>
   <si>
     <t xml:space="preserve">aaaaaaaaaaaaaaaa</t>
@@ -223,10 +238,13 @@
     <t xml:space="preserve">aaaaaaaaaaaaaaaaa</t>
   </si>
   <si>
+    <t xml:space="preserve">lat/lng: (12.6175727,0.8987057)</t>
+  </si>
+  <si>
     <t xml:space="preserve">aaaaaaaaaaaaaaaaaa</t>
   </si>
   <si>
-    <t xml:space="preserve">lat/lng: (23.6175727,9.8987057)</t>
+    <t xml:space="preserve">lat/lng: (23.6175727,10.8987057)</t>
   </si>
   <si>
     <t xml:space="preserve">aaaaaaaaaaaaaaaaaaa</t>
@@ -235,12 +253,15 @@
     <t xml:space="preserve">aaaaaaaaaaaaaaaaaaaa</t>
   </si>
   <si>
-    <t xml:space="preserve">lat/lng: (43.7175727,9.8987057)</t>
+    <t xml:space="preserve">lat/lng: (43.7175727,16.8987057)</t>
   </si>
   <si>
     <t xml:space="preserve">aaaaaaaaaaaaaaaaaaaaa</t>
   </si>
   <si>
+    <t xml:space="preserve">lat/lng: (53.6175727,17.8987057)</t>
+  </si>
+  <si>
     <t xml:space="preserve">aaaaaaaaaaaaaaaaaaaaaa</t>
   </si>
   <si>
@@ -248,6 +269,15 @@
   </si>
   <si>
     <t xml:space="preserve">aaaaaaaaaaaaaaaaaaaaaaaa</t>
+  </si>
+  <si>
+    <t>runningrain;3_5streak;2_10streak;2_</t>
+  </si>
+  <si>
+    <t>runningrain;3_5streak;2_10streak;3_</t>
+  </si>
+  <si>
+    <t>runningrain;3_5streak;2_10streak;4_</t>
   </si>
 </sst>
 </file>
@@ -337,7 +367,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -355,6 +385,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -377,30 +411,31 @@
   </sheetPr>
   <dimension ref="A1:AY35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q9" activeCellId="0" sqref="Q9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="36.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="31.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="32.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="21.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="14.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="17.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="18.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="23.76"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="11.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="15.18"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="18" style="1" width="11.67"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="36.54" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="31.68" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="30.97" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="31.12" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="1" width="8.75" collapsed="true" outlineLevel="0"/>
+    <col min="6" max="6" customWidth="true" hidden="false" style="1" width="17.92" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="7" customWidth="true" hidden="false" style="1" width="16.87" collapsed="true" outlineLevel="0"/>
+    <col min="8" max="8" customWidth="true" hidden="false" style="1" width="32.22" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="21.95" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="14.43" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="1" width="14.21" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="17.52" collapsed="true" outlineLevel="0"/>
+    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="18.77" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="true" hidden="false" style="1" width="16.81" collapsed="true" outlineLevel="0"/>
+    <col min="15" max="15" customWidth="true" hidden="false" style="1" width="23.76" collapsed="true" outlineLevel="0"/>
+    <col min="16" max="16" customWidth="false" hidden="false" style="1" width="11.67" collapsed="true" outlineLevel="0"/>
+    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="15.18" collapsed="true" outlineLevel="0"/>
+    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="36.12" collapsed="true" outlineLevel="0"/>
+    <col min="19" max="1025" customWidth="false" hidden="false" style="1" width="11.67" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -455,7 +490,9 @@
       <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3"/>
+      <c r="R1" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
       <c r="U1" s="3"/>
@@ -470,941 +507,949 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K2" s="0"/>
+      <c r="L2" t="s">
+        <v>85</v>
+      </c>
       <c r="N2" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="AY2" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K3" s="0"/>
       <c r="N3" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="AY3" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="J4" s="5"/>
       <c r="K4" s="0"/>
       <c r="N4" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="AY4" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K5" s="0"/>
       <c r="N5" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="AY5" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N6" s="4"/>
       <c r="Q6" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="AY6" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="J27" s="5"/>
       <c r="N27" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
changed the way medals were saved
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="87">
   <si>
     <t xml:space="preserve">Username</t>
   </si>
@@ -103,7 +103,7 @@
     <t xml:space="preserve">R.mipmap.avatar1 </t>
   </si>
   <si>
-    <t xml:space="preserve">5streak;2_10streak;4_runningrain;4_</t>
+    <t xml:space="preserve">5streak;2-10streak;4-runningrain;4-</t>
   </si>
   <si>
     <t xml:space="preserve">0</t>
@@ -278,6 +278,9 @@
   </si>
   <si>
     <t xml:space="preserve">aaaaaaaaaaaaaaaaaaaaaaaa</t>
+  </si>
+  <si>
+    <t>5streak;2-runningrain;4-10streak;5-</t>
   </si>
 </sst>
 </file>
@@ -411,31 +414,31 @@
   </sheetPr>
   <dimension ref="A1:AY35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J22" activeCellId="0" sqref="J22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M10" activeCellId="0" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="36.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="31.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="32.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="21.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="14.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="17.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="18.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="23.76"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="11.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="15.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="36.12"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="19" style="1" width="11.67"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="36.54" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="31.68" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="30.97" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="31.12" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="1" width="8.75" collapsed="true" outlineLevel="0"/>
+    <col min="6" max="6" customWidth="true" hidden="false" style="1" width="17.92" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="7" customWidth="true" hidden="false" style="1" width="16.87" collapsed="true" outlineLevel="0"/>
+    <col min="8" max="8" customWidth="true" hidden="false" style="1" width="32.22" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="21.95" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="14.43" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="1" width="14.21" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="17.52" collapsed="true" outlineLevel="0"/>
+    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="18.77" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="true" hidden="false" style="1" width="16.81" collapsed="true" outlineLevel="0"/>
+    <col min="15" max="15" customWidth="true" hidden="false" style="1" width="23.76" collapsed="true" outlineLevel="0"/>
+    <col min="16" max="16" customWidth="false" hidden="false" style="1" width="11.67" collapsed="true" outlineLevel="0"/>
+    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="15.18" collapsed="true" outlineLevel="0"/>
+    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="36.12" collapsed="true" outlineLevel="0"/>
+    <col min="19" max="1025" customWidth="false" hidden="false" style="1" width="11.67" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -533,8 +536,8 @@
       <c r="K2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>27</v>
+      <c r="L2" t="s">
+        <v>86</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
added a "getallusers" command
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="89">
   <si>
     <t xml:space="preserve">Username</t>
   </si>
@@ -287,12 +287,6 @@
   </si>
   <si>
     <t xml:space="preserve">aaaaaaaaaaaaaaaaaaaaaaaa</t>
-  </si>
-  <si>
-    <t>lat/lng: (53.6175727,9.8987057)</t>
-  </si>
-  <si>
-    <t>lat/lng: (50)</t>
   </si>
 </sst>
 </file>
@@ -427,30 +421,30 @@
   <dimension ref="A1:AY35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O69" activeCellId="0" sqref="O69"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="1" width="36.54" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="1" width="31.68" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="3" customWidth="true" hidden="false" style="1" width="30.97" collapsed="true" outlineLevel="0"/>
-    <col min="4" max="4" customWidth="true" hidden="false" style="1" width="31.12" collapsed="true" outlineLevel="0"/>
-    <col min="5" max="5" customWidth="true" hidden="false" style="1" width="8.75" collapsed="true" outlineLevel="0"/>
-    <col min="6" max="6" customWidth="true" hidden="false" style="1" width="17.92" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="7" customWidth="true" hidden="false" style="1" width="16.87" collapsed="true" outlineLevel="0"/>
-    <col min="8" max="8" customWidth="true" hidden="false" style="1" width="32.22" collapsed="true" outlineLevel="0"/>
-    <col min="9" max="9" customWidth="true" hidden="false" style="1" width="21.95" collapsed="true" outlineLevel="0"/>
-    <col min="10" max="10" customWidth="true" hidden="false" style="1" width="14.43" collapsed="true" outlineLevel="0"/>
-    <col min="11" max="11" customWidth="true" hidden="false" style="1" width="14.21" collapsed="true" outlineLevel="0"/>
-    <col min="12" max="12" customWidth="true" hidden="false" style="1" width="17.52" collapsed="true" outlineLevel="0"/>
-    <col min="13" max="13" customWidth="true" hidden="false" style="1" width="18.77" collapsed="true" outlineLevel="0"/>
-    <col min="14" max="14" customWidth="true" hidden="false" style="1" width="16.81" collapsed="true" outlineLevel="0"/>
-    <col min="15" max="15" customWidth="true" hidden="false" style="1" width="23.76" collapsed="true" outlineLevel="0"/>
-    <col min="16" max="16" customWidth="false" hidden="false" style="1" width="11.67" collapsed="true" outlineLevel="0"/>
-    <col min="17" max="17" customWidth="true" hidden="false" style="1" width="15.18" collapsed="true" outlineLevel="0"/>
-    <col min="18" max="18" customWidth="true" hidden="false" style="1" width="36.12" collapsed="true" outlineLevel="0"/>
-    <col min="19" max="1025" customWidth="false" hidden="false" style="1" width="11.67" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="36.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="31.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="32.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="21.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="14.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="17.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="18.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="23.76"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="11.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="15.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="36.12"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="19" style="1" width="11.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -542,8 +536,8 @@
       <c r="G2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H2" t="s">
-        <v>89</v>
+      <c r="H2" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>26</v>

</xml_diff>